<commit_message>
Tooltip issue css fixed, upload status tooltip lineitem added instead of production order no, upload status excel format changed, save -submit disabled issue fixed
</commit_message>
<xml_diff>
--- a/src/assets/data/uploadstatusFormat.xlsx
+++ b/src/assets/data/uploadstatusFormat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lapp\Production\lapp\src\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lapp New Cloned 03.02.20\lapp\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AF701A-5A33-400B-B956-E2EA67E63D09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE0DE24-657A-4C87-9219-16D575AB6B4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AE4E98DC-39C1-491B-B890-75172FA0A1A2}"/>
   </bookViews>
@@ -35,10 +35,10 @@
     <t>SalesOrder No</t>
   </si>
   <si>
-    <t>ProductionOrder No</t>
+    <t>Status</t>
   </si>
   <si>
-    <t>Status</t>
+    <t>LineItem</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,10 +430,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="3"/>
     </row>

</xml_diff>